<commit_message>
changed current sense amplifier
</commit_message>
<xml_diff>
--- a/BOM_rev1_v3.xlsx
+++ b/BOM_rev1_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliow\OneDrive\Dokumente\GitHub\CHESS_OBC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57e57102d9b92534/Dokumente/GitHub/CHESS_OBC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B077D1-6D78-456F-B5E9-7A4FEED4016A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{35B077D1-6D78-456F-B5E9-7A4FEED4016A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{139DB1A0-6A7E-4A22-BDF0-E06E46474BC6}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4800" yWindow="3128" windowWidth="14400" windowHeight="8272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="1515" windowWidth="14400" windowHeight="8273" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBC-Components" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="204">
   <si>
     <t>Designator</t>
   </si>
@@ -552,19 +552,7 @@
     <t>FPGA</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>LT6105IMS8#PBF</t>
-  </si>
-  <si>
     <t>Current Sense Amplifier</t>
-  </si>
-  <si>
-    <t>Stromfühler-Verstärker LT6105IMS8#PBF, Single Differential MSOP 8-Pin | RS Components (rs-online.com)</t>
-  </si>
-  <si>
-    <t>9 in stock</t>
   </si>
   <si>
     <t>LM3671MF-3.3/NOPB</t>
@@ -651,6 +639,12 @@
   <si>
     <t>ESQ-126-39-G-D</t>
   </si>
+  <si>
+    <t>CurrentSensing</t>
+  </si>
+  <si>
+    <t>INA138QPWRQ1</t>
+  </si>
 </sst>
 </file>
 
@@ -659,7 +653,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$Fr.-807]\ #,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -723,12 +717,6 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
@@ -745,7 +733,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,18 +752,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
-        <bgColor rgb="FFFFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -788,9 +764,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -819,14 +795,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1048,8 +1022,8 @@
   </sheetPr>
   <dimension ref="A1:AD995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1428,11 +1402,11 @@
       <c r="AD7" s="8"/>
     </row>
     <row r="8" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
@@ -1446,7 +1420,7 @@
       <c r="F8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="15"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
@@ -1474,11 +1448,11 @@
       <c r="AD8" s="12"/>
     </row>
     <row r="9" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>197</v>
+      <c r="B9" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -1495,11 +1469,11 @@
       <c r="G9" s="16">
         <v>0.69</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>198</v>
+      <c r="H9" s="24" t="s">
+        <v>194</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>199</v>
+      <c r="I9" s="25" t="s">
+        <v>195</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1575,7 +1549,7 @@
     </row>
     <row r="11" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>64</v>
@@ -1672,11 +1646,11 @@
       <c r="AD12" s="8"/>
     </row>
     <row r="13" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>205</v>
+      <c r="B13" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="C13" s="13">
         <v>2</v>
@@ -1715,7 +1689,7 @@
     </row>
     <row r="14" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>77</v>
@@ -1863,7 +1837,7 @@
     </row>
     <row r="17" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>93</v>
@@ -1959,10 +1933,10 @@
     </row>
     <row r="19" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>200</v>
+      <c r="B19" s="23" t="s">
+        <v>196</v>
       </c>
       <c r="C19" s="13">
         <v>1</v>
@@ -1979,11 +1953,11 @@
       <c r="G19" s="16">
         <v>0.77</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>202</v>
+      <c r="H19" s="24" t="s">
+        <v>198</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>201</v>
+      <c r="I19" s="25" t="s">
+        <v>197</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -2665,8 +2639,8 @@
       <c r="A33" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>203</v>
+      <c r="B33" s="23" t="s">
+        <v>199</v>
       </c>
       <c r="C33" s="13">
         <v>1</v>
@@ -2674,8 +2648,8 @@
       <c r="D33" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E33" s="26" t="s">
-        <v>203</v>
+      <c r="E33" s="25" t="s">
+        <v>199</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="16"/>
@@ -2705,30 +2679,24 @@
     </row>
     <row r="34" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="C34" s="13">
         <v>1</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="18">
-        <v>2.8</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>177</v>
-      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -2753,29 +2721,29 @@
     </row>
     <row r="35" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C35" s="13">
         <v>1</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="16">
         <v>1.52</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -2800,11 +2768,11 @@
       <c r="AD35" s="8"/>
     </row>
     <row r="36" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A36" s="23" t="s">
-        <v>194</v>
+      <c r="A36" s="22" t="s">
+        <v>190</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C36" s="7">
         <v>1</v>
@@ -2813,19 +2781,19 @@
         <v>54</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G36" s="16">
         <v>0.82</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2851,29 +2819,29 @@
     </row>
     <row r="37" spans="1:30" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C37" s="13">
         <v>1</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="16">
         <v>1.87</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2904,7 +2872,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="21"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -2934,7 +2902,7 @@
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="22"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="16"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
@@ -2967,7 +2935,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="21"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -2999,7 +2967,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -3031,7 +2999,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="21"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -3063,7 +3031,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="21"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -3095,7 +3063,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -3127,7 +3095,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="21"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
@@ -3159,7 +3127,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="21"/>
+      <c r="G46" s="20"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
@@ -3191,7 +3159,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="21"/>
+      <c r="G47" s="20"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
@@ -3223,7 +3191,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="21"/>
+      <c r="G48" s="20"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
@@ -3255,7 +3223,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
-      <c r="G49" s="21"/>
+      <c r="G49" s="20"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
@@ -3287,7 +3255,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="21"/>
+      <c r="G50" s="20"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -3319,7 +3287,7 @@
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
-      <c r="G51" s="21"/>
+      <c r="G51" s="20"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
@@ -3351,7 +3319,7 @@
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
-      <c r="G52" s="21"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
@@ -3383,7 +3351,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
-      <c r="G53" s="21"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
@@ -3415,7 +3383,7 @@
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="21"/>
+      <c r="G54" s="20"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -3447,7 +3415,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
-      <c r="G55" s="21"/>
+      <c r="G55" s="20"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
@@ -3479,7 +3447,7 @@
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
-      <c r="G56" s="21"/>
+      <c r="G56" s="20"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -3511,7 +3479,7 @@
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
-      <c r="G57" s="21"/>
+      <c r="G57" s="20"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
@@ -3543,7 +3511,7 @@
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
-      <c r="G58" s="21"/>
+      <c r="G58" s="20"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -3575,7 +3543,7 @@
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
-      <c r="G59" s="21"/>
+      <c r="G59" s="20"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
@@ -3607,7 +3575,7 @@
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
-      <c r="G60" s="21"/>
+      <c r="G60" s="20"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -3639,7 +3607,7 @@
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
-      <c r="G61" s="21"/>
+      <c r="G61" s="20"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
@@ -3671,7 +3639,7 @@
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
-      <c r="G62" s="21"/>
+      <c r="G62" s="20"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -3703,7 +3671,7 @@
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
-      <c r="G63" s="21"/>
+      <c r="G63" s="20"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
@@ -3735,7 +3703,7 @@
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
-      <c r="G64" s="21"/>
+      <c r="G64" s="20"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
@@ -3767,7 +3735,7 @@
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
-      <c r="G65" s="21"/>
+      <c r="G65" s="20"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
@@ -3799,7 +3767,7 @@
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
-      <c r="G66" s="21"/>
+      <c r="G66" s="20"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
@@ -3831,7 +3799,7 @@
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
-      <c r="G67" s="21"/>
+      <c r="G67" s="20"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
       <c r="J67" s="8"/>
@@ -3863,7 +3831,7 @@
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
-      <c r="G68" s="21"/>
+      <c r="G68" s="20"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
@@ -3895,7 +3863,7 @@
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
-      <c r="G69" s="21"/>
+      <c r="G69" s="20"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
       <c r="J69" s="8"/>
@@ -3927,7 +3895,7 @@
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
-      <c r="G70" s="21"/>
+      <c r="G70" s="20"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
@@ -3959,7 +3927,7 @@
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
-      <c r="G71" s="21"/>
+      <c r="G71" s="20"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="8"/>
@@ -3991,7 +3959,7 @@
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="21"/>
+      <c r="G72" s="20"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
@@ -4023,7 +3991,7 @@
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
-      <c r="G73" s="21"/>
+      <c r="G73" s="20"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
       <c r="J73" s="8"/>
@@ -4055,7 +4023,7 @@
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
-      <c r="G74" s="21"/>
+      <c r="G74" s="20"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
@@ -4087,7 +4055,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
-      <c r="G75" s="21"/>
+      <c r="G75" s="20"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="8"/>
@@ -4119,7 +4087,7 @@
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
-      <c r="G76" s="21"/>
+      <c r="G76" s="20"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
@@ -4151,7 +4119,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="21"/>
+      <c r="G77" s="20"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
       <c r="J77" s="8"/>
@@ -4183,7 +4151,7 @@
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
-      <c r="G78" s="21"/>
+      <c r="G78" s="20"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
@@ -4215,7 +4183,7 @@
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
-      <c r="G79" s="21"/>
+      <c r="G79" s="20"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
       <c r="J79" s="8"/>
@@ -4247,7 +4215,7 @@
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
-      <c r="G80" s="21"/>
+      <c r="G80" s="20"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
@@ -4279,7 +4247,7 @@
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
-      <c r="G81" s="21"/>
+      <c r="G81" s="20"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
@@ -4311,7 +4279,7 @@
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
-      <c r="G82" s="21"/>
+      <c r="G82" s="20"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
@@ -4343,7 +4311,7 @@
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
-      <c r="G83" s="21"/>
+      <c r="G83" s="20"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -4375,7 +4343,7 @@
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
-      <c r="G84" s="21"/>
+      <c r="G84" s="20"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
@@ -4407,7 +4375,7 @@
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
       <c r="F85" s="8"/>
-      <c r="G85" s="21"/>
+      <c r="G85" s="20"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -4439,7 +4407,7 @@
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
-      <c r="G86" s="21"/>
+      <c r="G86" s="20"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
@@ -4471,7 +4439,7 @@
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
-      <c r="G87" s="21"/>
+      <c r="G87" s="20"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -4503,7 +4471,7 @@
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
-      <c r="G88" s="21"/>
+      <c r="G88" s="20"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
@@ -4535,7 +4503,7 @@
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
-      <c r="G89" s="21"/>
+      <c r="G89" s="20"/>
       <c r="H89" s="8"/>
       <c r="I89" s="8"/>
       <c r="J89" s="8"/>
@@ -4567,7 +4535,7 @@
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
       <c r="F90" s="8"/>
-      <c r="G90" s="21"/>
+      <c r="G90" s="20"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -4599,7 +4567,7 @@
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
       <c r="F91" s="8"/>
-      <c r="G91" s="21"/>
+      <c r="G91" s="20"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
       <c r="J91" s="8"/>
@@ -4631,7 +4599,7 @@
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
-      <c r="G92" s="21"/>
+      <c r="G92" s="20"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
@@ -4663,7 +4631,7 @@
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
-      <c r="G93" s="21"/>
+      <c r="G93" s="20"/>
       <c r="H93" s="8"/>
       <c r="I93" s="8"/>
       <c r="J93" s="8"/>
@@ -4695,7 +4663,7 @@
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
-      <c r="G94" s="21"/>
+      <c r="G94" s="20"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
@@ -4727,7 +4695,7 @@
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
       <c r="F95" s="8"/>
-      <c r="G95" s="21"/>
+      <c r="G95" s="20"/>
       <c r="H95" s="8"/>
       <c r="I95" s="8"/>
       <c r="J95" s="8"/>
@@ -4759,7 +4727,7 @@
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
-      <c r="G96" s="21"/>
+      <c r="G96" s="20"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="8"/>
@@ -4791,7 +4759,7 @@
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
-      <c r="G97" s="21"/>
+      <c r="G97" s="20"/>
       <c r="H97" s="8"/>
       <c r="I97" s="8"/>
       <c r="J97" s="8"/>
@@ -4823,7 +4791,7 @@
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
       <c r="F98" s="8"/>
-      <c r="G98" s="21"/>
+      <c r="G98" s="20"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
@@ -4855,7 +4823,7 @@
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
-      <c r="G99" s="21"/>
+      <c r="G99" s="20"/>
       <c r="H99" s="8"/>
       <c r="I99" s="8"/>
       <c r="J99" s="8"/>
@@ -4887,7 +4855,7 @@
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
-      <c r="G100" s="21"/>
+      <c r="G100" s="20"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
@@ -4919,7 +4887,7 @@
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
       <c r="F101" s="8"/>
-      <c r="G101" s="21"/>
+      <c r="G101" s="20"/>
       <c r="H101" s="8"/>
       <c r="I101" s="8"/>
       <c r="J101" s="8"/>
@@ -4951,7 +4919,7 @@
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
-      <c r="G102" s="21"/>
+      <c r="G102" s="20"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
@@ -4983,7 +4951,7 @@
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
-      <c r="G103" s="21"/>
+      <c r="G103" s="20"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
       <c r="J103" s="8"/>
@@ -5015,7 +4983,7 @@
       <c r="D104" s="8"/>
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
-      <c r="G104" s="21"/>
+      <c r="G104" s="20"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
@@ -5047,7 +5015,7 @@
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
-      <c r="G105" s="21"/>
+      <c r="G105" s="20"/>
       <c r="H105" s="8"/>
       <c r="I105" s="8"/>
       <c r="J105" s="8"/>
@@ -5079,7 +5047,7 @@
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
-      <c r="G106" s="21"/>
+      <c r="G106" s="20"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
@@ -5111,7 +5079,7 @@
       <c r="D107" s="8"/>
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
-      <c r="G107" s="21"/>
+      <c r="G107" s="20"/>
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
       <c r="J107" s="8"/>
@@ -5143,7 +5111,7 @@
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
-      <c r="G108" s="21"/>
+      <c r="G108" s="20"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
@@ -5175,7 +5143,7 @@
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
-      <c r="G109" s="21"/>
+      <c r="G109" s="20"/>
       <c r="H109" s="8"/>
       <c r="I109" s="8"/>
       <c r="J109" s="8"/>
@@ -5207,7 +5175,7 @@
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
-      <c r="G110" s="21"/>
+      <c r="G110" s="20"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
@@ -5239,7 +5207,7 @@
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
-      <c r="G111" s="21"/>
+      <c r="G111" s="20"/>
       <c r="H111" s="8"/>
       <c r="I111" s="8"/>
       <c r="J111" s="8"/>
@@ -5271,7 +5239,7 @@
       <c r="D112" s="8"/>
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
-      <c r="G112" s="21"/>
+      <c r="G112" s="20"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
       <c r="J112" s="8"/>
@@ -5303,7 +5271,7 @@
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
-      <c r="G113" s="21"/>
+      <c r="G113" s="20"/>
       <c r="H113" s="8"/>
       <c r="I113" s="8"/>
       <c r="J113" s="8"/>
@@ -5335,7 +5303,7 @@
       <c r="D114" s="8"/>
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
-      <c r="G114" s="21"/>
+      <c r="G114" s="20"/>
       <c r="H114" s="8"/>
       <c r="I114" s="8"/>
       <c r="J114" s="8"/>
@@ -5367,7 +5335,7 @@
       <c r="D115" s="8"/>
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
-      <c r="G115" s="21"/>
+      <c r="G115" s="20"/>
       <c r="H115" s="8"/>
       <c r="I115" s="8"/>
       <c r="J115" s="8"/>
@@ -5399,7 +5367,7 @@
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
-      <c r="G116" s="21"/>
+      <c r="G116" s="20"/>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
       <c r="J116" s="8"/>
@@ -5431,7 +5399,7 @@
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
-      <c r="G117" s="21"/>
+      <c r="G117" s="20"/>
       <c r="H117" s="8"/>
       <c r="I117" s="8"/>
       <c r="J117" s="8"/>
@@ -5463,7 +5431,7 @@
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
-      <c r="G118" s="21"/>
+      <c r="G118" s="20"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="8"/>
@@ -5495,7 +5463,7 @@
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
-      <c r="G119" s="21"/>
+      <c r="G119" s="20"/>
       <c r="H119" s="8"/>
       <c r="I119" s="8"/>
       <c r="J119" s="8"/>
@@ -5527,7 +5495,7 @@
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
-      <c r="G120" s="21"/>
+      <c r="G120" s="20"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
@@ -5559,7 +5527,7 @@
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
-      <c r="G121" s="21"/>
+      <c r="G121" s="20"/>
       <c r="H121" s="8"/>
       <c r="I121" s="8"/>
       <c r="J121" s="8"/>
@@ -5591,7 +5559,7 @@
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
-      <c r="G122" s="21"/>
+      <c r="G122" s="20"/>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
@@ -5623,7 +5591,7 @@
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
-      <c r="G123" s="21"/>
+      <c r="G123" s="20"/>
       <c r="H123" s="8"/>
       <c r="I123" s="8"/>
       <c r="J123" s="8"/>
@@ -5655,7 +5623,7 @@
       <c r="D124" s="8"/>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
-      <c r="G124" s="21"/>
+      <c r="G124" s="20"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
@@ -5687,7 +5655,7 @@
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
-      <c r="G125" s="21"/>
+      <c r="G125" s="20"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="8"/>
@@ -5719,7 +5687,7 @@
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
-      <c r="G126" s="21"/>
+      <c r="G126" s="20"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>
@@ -5751,7 +5719,7 @@
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
-      <c r="G127" s="21"/>
+      <c r="G127" s="20"/>
       <c r="H127" s="8"/>
       <c r="I127" s="8"/>
       <c r="J127" s="8"/>
@@ -5783,7 +5751,7 @@
       <c r="D128" s="8"/>
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
-      <c r="G128" s="21"/>
+      <c r="G128" s="20"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="8"/>
@@ -5815,7 +5783,7 @@
       <c r="D129" s="8"/>
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
-      <c r="G129" s="21"/>
+      <c r="G129" s="20"/>
       <c r="H129" s="8"/>
       <c r="I129" s="8"/>
       <c r="J129" s="8"/>
@@ -5847,7 +5815,7 @@
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
-      <c r="G130" s="21"/>
+      <c r="G130" s="20"/>
       <c r="H130" s="8"/>
       <c r="I130" s="8"/>
       <c r="J130" s="8"/>
@@ -5879,7 +5847,7 @@
       <c r="D131" s="8"/>
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
-      <c r="G131" s="21"/>
+      <c r="G131" s="20"/>
       <c r="H131" s="8"/>
       <c r="I131" s="8"/>
       <c r="J131" s="8"/>
@@ -5911,7 +5879,7 @@
       <c r="D132" s="8"/>
       <c r="E132" s="8"/>
       <c r="F132" s="8"/>
-      <c r="G132" s="21"/>
+      <c r="G132" s="20"/>
       <c r="H132" s="8"/>
       <c r="I132" s="8"/>
       <c r="J132" s="8"/>
@@ -5943,7 +5911,7 @@
       <c r="D133" s="8"/>
       <c r="E133" s="8"/>
       <c r="F133" s="8"/>
-      <c r="G133" s="21"/>
+      <c r="G133" s="20"/>
       <c r="H133" s="8"/>
       <c r="I133" s="8"/>
       <c r="J133" s="8"/>
@@ -5975,7 +5943,7 @@
       <c r="D134" s="8"/>
       <c r="E134" s="8"/>
       <c r="F134" s="8"/>
-      <c r="G134" s="21"/>
+      <c r="G134" s="20"/>
       <c r="H134" s="8"/>
       <c r="I134" s="8"/>
       <c r="J134" s="8"/>
@@ -6007,7 +5975,7 @@
       <c r="D135" s="8"/>
       <c r="E135" s="8"/>
       <c r="F135" s="8"/>
-      <c r="G135" s="21"/>
+      <c r="G135" s="20"/>
       <c r="H135" s="8"/>
       <c r="I135" s="8"/>
       <c r="J135" s="8"/>
@@ -6039,7 +6007,7 @@
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
       <c r="F136" s="8"/>
-      <c r="G136" s="21"/>
+      <c r="G136" s="20"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
@@ -6071,7 +6039,7 @@
       <c r="D137" s="8"/>
       <c r="E137" s="8"/>
       <c r="F137" s="8"/>
-      <c r="G137" s="21"/>
+      <c r="G137" s="20"/>
       <c r="H137" s="8"/>
       <c r="I137" s="8"/>
       <c r="J137" s="8"/>
@@ -6103,7 +6071,7 @@
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
-      <c r="G138" s="21"/>
+      <c r="G138" s="20"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
@@ -6135,7 +6103,7 @@
       <c r="D139" s="8"/>
       <c r="E139" s="8"/>
       <c r="F139" s="8"/>
-      <c r="G139" s="21"/>
+      <c r="G139" s="20"/>
       <c r="H139" s="8"/>
       <c r="I139" s="8"/>
       <c r="J139" s="8"/>
@@ -6167,7 +6135,7 @@
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
-      <c r="G140" s="21"/>
+      <c r="G140" s="20"/>
       <c r="H140" s="8"/>
       <c r="I140" s="8"/>
       <c r="J140" s="8"/>
@@ -6199,7 +6167,7 @@
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
-      <c r="G141" s="21"/>
+      <c r="G141" s="20"/>
       <c r="H141" s="8"/>
       <c r="I141" s="8"/>
       <c r="J141" s="8"/>
@@ -6231,7 +6199,7 @@
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
       <c r="F142" s="8"/>
-      <c r="G142" s="21"/>
+      <c r="G142" s="20"/>
       <c r="H142" s="8"/>
       <c r="I142" s="8"/>
       <c r="J142" s="8"/>
@@ -6263,7 +6231,7 @@
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
       <c r="F143" s="8"/>
-      <c r="G143" s="21"/>
+      <c r="G143" s="20"/>
       <c r="H143" s="8"/>
       <c r="I143" s="8"/>
       <c r="J143" s="8"/>
@@ -6295,7 +6263,7 @@
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
-      <c r="G144" s="21"/>
+      <c r="G144" s="20"/>
       <c r="H144" s="8"/>
       <c r="I144" s="8"/>
       <c r="J144" s="8"/>
@@ -6327,7 +6295,7 @@
       <c r="D145" s="8"/>
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
-      <c r="G145" s="21"/>
+      <c r="G145" s="20"/>
       <c r="H145" s="8"/>
       <c r="I145" s="8"/>
       <c r="J145" s="8"/>
@@ -6359,7 +6327,7 @@
       <c r="D146" s="8"/>
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
-      <c r="G146" s="21"/>
+      <c r="G146" s="20"/>
       <c r="H146" s="8"/>
       <c r="I146" s="8"/>
       <c r="J146" s="8"/>
@@ -6391,7 +6359,7 @@
       <c r="D147" s="8"/>
       <c r="E147" s="8"/>
       <c r="F147" s="8"/>
-      <c r="G147" s="21"/>
+      <c r="G147" s="20"/>
       <c r="H147" s="8"/>
       <c r="I147" s="8"/>
       <c r="J147" s="8"/>
@@ -6423,7 +6391,7 @@
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
       <c r="F148" s="8"/>
-      <c r="G148" s="21"/>
+      <c r="G148" s="20"/>
       <c r="H148" s="8"/>
       <c r="I148" s="8"/>
       <c r="J148" s="8"/>
@@ -6455,7 +6423,7 @@
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
       <c r="F149" s="8"/>
-      <c r="G149" s="21"/>
+      <c r="G149" s="20"/>
       <c r="H149" s="8"/>
       <c r="I149" s="8"/>
       <c r="J149" s="8"/>
@@ -6487,7 +6455,7 @@
       <c r="D150" s="8"/>
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
-      <c r="G150" s="21"/>
+      <c r="G150" s="20"/>
       <c r="H150" s="8"/>
       <c r="I150" s="8"/>
       <c r="J150" s="8"/>
@@ -6519,7 +6487,7 @@
       <c r="D151" s="8"/>
       <c r="E151" s="8"/>
       <c r="F151" s="8"/>
-      <c r="G151" s="21"/>
+      <c r="G151" s="20"/>
       <c r="H151" s="8"/>
       <c r="I151" s="8"/>
       <c r="J151" s="8"/>
@@ -6551,7 +6519,7 @@
       <c r="D152" s="8"/>
       <c r="E152" s="8"/>
       <c r="F152" s="8"/>
-      <c r="G152" s="21"/>
+      <c r="G152" s="20"/>
       <c r="H152" s="8"/>
       <c r="I152" s="8"/>
       <c r="J152" s="8"/>
@@ -6583,7 +6551,7 @@
       <c r="D153" s="8"/>
       <c r="E153" s="8"/>
       <c r="F153" s="8"/>
-      <c r="G153" s="21"/>
+      <c r="G153" s="20"/>
       <c r="H153" s="8"/>
       <c r="I153" s="8"/>
       <c r="J153" s="8"/>
@@ -6615,7 +6583,7 @@
       <c r="D154" s="8"/>
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
-      <c r="G154" s="21"/>
+      <c r="G154" s="20"/>
       <c r="H154" s="8"/>
       <c r="I154" s="8"/>
       <c r="J154" s="8"/>
@@ -6647,7 +6615,7 @@
       <c r="D155" s="8"/>
       <c r="E155" s="8"/>
       <c r="F155" s="8"/>
-      <c r="G155" s="21"/>
+      <c r="G155" s="20"/>
       <c r="H155" s="8"/>
       <c r="I155" s="8"/>
       <c r="J155" s="8"/>
@@ -6679,7 +6647,7 @@
       <c r="D156" s="8"/>
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
-      <c r="G156" s="21"/>
+      <c r="G156" s="20"/>
       <c r="H156" s="8"/>
       <c r="I156" s="8"/>
       <c r="J156" s="8"/>
@@ -6711,7 +6679,7 @@
       <c r="D157" s="8"/>
       <c r="E157" s="8"/>
       <c r="F157" s="8"/>
-      <c r="G157" s="21"/>
+      <c r="G157" s="20"/>
       <c r="H157" s="8"/>
       <c r="I157" s="8"/>
       <c r="J157" s="8"/>
@@ -6743,7 +6711,7 @@
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
       <c r="F158" s="8"/>
-      <c r="G158" s="21"/>
+      <c r="G158" s="20"/>
       <c r="H158" s="8"/>
       <c r="I158" s="8"/>
       <c r="J158" s="8"/>
@@ -6775,7 +6743,7 @@
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
       <c r="F159" s="8"/>
-      <c r="G159" s="21"/>
+      <c r="G159" s="20"/>
       <c r="H159" s="8"/>
       <c r="I159" s="8"/>
       <c r="J159" s="8"/>
@@ -6807,7 +6775,7 @@
       <c r="D160" s="8"/>
       <c r="E160" s="8"/>
       <c r="F160" s="8"/>
-      <c r="G160" s="21"/>
+      <c r="G160" s="20"/>
       <c r="H160" s="8"/>
       <c r="I160" s="8"/>
       <c r="J160" s="8"/>
@@ -6839,7 +6807,7 @@
       <c r="D161" s="8"/>
       <c r="E161" s="8"/>
       <c r="F161" s="8"/>
-      <c r="G161" s="21"/>
+      <c r="G161" s="20"/>
       <c r="H161" s="8"/>
       <c r="I161" s="8"/>
       <c r="J161" s="8"/>
@@ -6871,7 +6839,7 @@
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
       <c r="F162" s="8"/>
-      <c r="G162" s="21"/>
+      <c r="G162" s="20"/>
       <c r="H162" s="8"/>
       <c r="I162" s="8"/>
       <c r="J162" s="8"/>
@@ -6903,7 +6871,7 @@
       <c r="D163" s="8"/>
       <c r="E163" s="8"/>
       <c r="F163" s="8"/>
-      <c r="G163" s="21"/>
+      <c r="G163" s="20"/>
       <c r="H163" s="8"/>
       <c r="I163" s="8"/>
       <c r="J163" s="8"/>
@@ -6935,7 +6903,7 @@
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
       <c r="F164" s="8"/>
-      <c r="G164" s="21"/>
+      <c r="G164" s="20"/>
       <c r="H164" s="8"/>
       <c r="I164" s="8"/>
       <c r="J164" s="8"/>
@@ -6967,7 +6935,7 @@
       <c r="D165" s="8"/>
       <c r="E165" s="8"/>
       <c r="F165" s="8"/>
-      <c r="G165" s="21"/>
+      <c r="G165" s="20"/>
       <c r="H165" s="8"/>
       <c r="I165" s="8"/>
       <c r="J165" s="8"/>
@@ -6999,7 +6967,7 @@
       <c r="D166" s="8"/>
       <c r="E166" s="8"/>
       <c r="F166" s="8"/>
-      <c r="G166" s="21"/>
+      <c r="G166" s="20"/>
       <c r="H166" s="8"/>
       <c r="I166" s="8"/>
       <c r="J166" s="8"/>
@@ -7031,7 +6999,7 @@
       <c r="D167" s="8"/>
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
-      <c r="G167" s="21"/>
+      <c r="G167" s="20"/>
       <c r="H167" s="8"/>
       <c r="I167" s="8"/>
       <c r="J167" s="8"/>
@@ -7063,7 +7031,7 @@
       <c r="D168" s="8"/>
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
-      <c r="G168" s="21"/>
+      <c r="G168" s="20"/>
       <c r="H168" s="8"/>
       <c r="I168" s="8"/>
       <c r="J168" s="8"/>
@@ -7095,7 +7063,7 @@
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
-      <c r="G169" s="21"/>
+      <c r="G169" s="20"/>
       <c r="H169" s="8"/>
       <c r="I169" s="8"/>
       <c r="J169" s="8"/>
@@ -7127,7 +7095,7 @@
       <c r="D170" s="8"/>
       <c r="E170" s="8"/>
       <c r="F170" s="8"/>
-      <c r="G170" s="21"/>
+      <c r="G170" s="20"/>
       <c r="H170" s="8"/>
       <c r="I170" s="8"/>
       <c r="J170" s="8"/>
@@ -7159,7 +7127,7 @@
       <c r="D171" s="8"/>
       <c r="E171" s="8"/>
       <c r="F171" s="8"/>
-      <c r="G171" s="21"/>
+      <c r="G171" s="20"/>
       <c r="H171" s="8"/>
       <c r="I171" s="8"/>
       <c r="J171" s="8"/>
@@ -7191,7 +7159,7 @@
       <c r="D172" s="8"/>
       <c r="E172" s="8"/>
       <c r="F172" s="8"/>
-      <c r="G172" s="21"/>
+      <c r="G172" s="20"/>
       <c r="H172" s="8"/>
       <c r="I172" s="8"/>
       <c r="J172" s="8"/>
@@ -7223,7 +7191,7 @@
       <c r="D173" s="8"/>
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
-      <c r="G173" s="21"/>
+      <c r="G173" s="20"/>
       <c r="H173" s="8"/>
       <c r="I173" s="8"/>
       <c r="J173" s="8"/>
@@ -7255,7 +7223,7 @@
       <c r="D174" s="8"/>
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
-      <c r="G174" s="21"/>
+      <c r="G174" s="20"/>
       <c r="H174" s="8"/>
       <c r="I174" s="8"/>
       <c r="J174" s="8"/>
@@ -7287,7 +7255,7 @@
       <c r="D175" s="8"/>
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
-      <c r="G175" s="21"/>
+      <c r="G175" s="20"/>
       <c r="H175" s="8"/>
       <c r="I175" s="8"/>
       <c r="J175" s="8"/>
@@ -7319,7 +7287,7 @@
       <c r="D176" s="8"/>
       <c r="E176" s="8"/>
       <c r="F176" s="8"/>
-      <c r="G176" s="21"/>
+      <c r="G176" s="20"/>
       <c r="H176" s="8"/>
       <c r="I176" s="8"/>
       <c r="J176" s="8"/>
@@ -7351,7 +7319,7 @@
       <c r="D177" s="8"/>
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
-      <c r="G177" s="21"/>
+      <c r="G177" s="20"/>
       <c r="H177" s="8"/>
       <c r="I177" s="8"/>
       <c r="J177" s="8"/>
@@ -7383,7 +7351,7 @@
       <c r="D178" s="8"/>
       <c r="E178" s="8"/>
       <c r="F178" s="8"/>
-      <c r="G178" s="21"/>
+      <c r="G178" s="20"/>
       <c r="H178" s="8"/>
       <c r="I178" s="8"/>
       <c r="J178" s="8"/>
@@ -7415,7 +7383,7 @@
       <c r="D179" s="8"/>
       <c r="E179" s="8"/>
       <c r="F179" s="8"/>
-      <c r="G179" s="21"/>
+      <c r="G179" s="20"/>
       <c r="H179" s="8"/>
       <c r="I179" s="8"/>
       <c r="J179" s="8"/>
@@ -7447,7 +7415,7 @@
       <c r="D180" s="8"/>
       <c r="E180" s="8"/>
       <c r="F180" s="8"/>
-      <c r="G180" s="21"/>
+      <c r="G180" s="20"/>
       <c r="H180" s="8"/>
       <c r="I180" s="8"/>
       <c r="J180" s="8"/>
@@ -7479,7 +7447,7 @@
       <c r="D181" s="8"/>
       <c r="E181" s="8"/>
       <c r="F181" s="8"/>
-      <c r="G181" s="21"/>
+      <c r="G181" s="20"/>
       <c r="H181" s="8"/>
       <c r="I181" s="8"/>
       <c r="J181" s="8"/>
@@ -7511,7 +7479,7 @@
       <c r="D182" s="8"/>
       <c r="E182" s="8"/>
       <c r="F182" s="8"/>
-      <c r="G182" s="21"/>
+      <c r="G182" s="20"/>
       <c r="H182" s="8"/>
       <c r="I182" s="8"/>
       <c r="J182" s="8"/>
@@ -7543,7 +7511,7 @@
       <c r="D183" s="8"/>
       <c r="E183" s="8"/>
       <c r="F183" s="8"/>
-      <c r="G183" s="21"/>
+      <c r="G183" s="20"/>
       <c r="H183" s="8"/>
       <c r="I183" s="8"/>
       <c r="J183" s="8"/>
@@ -7575,7 +7543,7 @@
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
       <c r="F184" s="8"/>
-      <c r="G184" s="21"/>
+      <c r="G184" s="20"/>
       <c r="H184" s="8"/>
       <c r="I184" s="8"/>
       <c r="J184" s="8"/>
@@ -7607,7 +7575,7 @@
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
       <c r="F185" s="8"/>
-      <c r="G185" s="21"/>
+      <c r="G185" s="20"/>
       <c r="H185" s="8"/>
       <c r="I185" s="8"/>
       <c r="J185" s="8"/>
@@ -7639,7 +7607,7 @@
       <c r="D186" s="8"/>
       <c r="E186" s="8"/>
       <c r="F186" s="8"/>
-      <c r="G186" s="21"/>
+      <c r="G186" s="20"/>
       <c r="H186" s="8"/>
       <c r="I186" s="8"/>
       <c r="J186" s="8"/>
@@ -7671,7 +7639,7 @@
       <c r="D187" s="8"/>
       <c r="E187" s="8"/>
       <c r="F187" s="8"/>
-      <c r="G187" s="21"/>
+      <c r="G187" s="20"/>
       <c r="H187" s="8"/>
       <c r="I187" s="8"/>
       <c r="J187" s="8"/>
@@ -7703,7 +7671,7 @@
       <c r="D188" s="8"/>
       <c r="E188" s="8"/>
       <c r="F188" s="8"/>
-      <c r="G188" s="21"/>
+      <c r="G188" s="20"/>
       <c r="H188" s="8"/>
       <c r="I188" s="8"/>
       <c r="J188" s="8"/>
@@ -7735,7 +7703,7 @@
       <c r="D189" s="8"/>
       <c r="E189" s="8"/>
       <c r="F189" s="8"/>
-      <c r="G189" s="21"/>
+      <c r="G189" s="20"/>
       <c r="H189" s="8"/>
       <c r="I189" s="8"/>
       <c r="J189" s="8"/>
@@ -7767,7 +7735,7 @@
       <c r="D190" s="8"/>
       <c r="E190" s="8"/>
       <c r="F190" s="8"/>
-      <c r="G190" s="21"/>
+      <c r="G190" s="20"/>
       <c r="H190" s="8"/>
       <c r="I190" s="8"/>
       <c r="J190" s="8"/>
@@ -7799,7 +7767,7 @@
       <c r="D191" s="8"/>
       <c r="E191" s="8"/>
       <c r="F191" s="8"/>
-      <c r="G191" s="21"/>
+      <c r="G191" s="20"/>
       <c r="H191" s="8"/>
       <c r="I191" s="8"/>
       <c r="J191" s="8"/>
@@ -7831,7 +7799,7 @@
       <c r="D192" s="8"/>
       <c r="E192" s="8"/>
       <c r="F192" s="8"/>
-      <c r="G192" s="21"/>
+      <c r="G192" s="20"/>
       <c r="H192" s="8"/>
       <c r="I192" s="8"/>
       <c r="J192" s="8"/>
@@ -7863,7 +7831,7 @@
       <c r="D193" s="8"/>
       <c r="E193" s="8"/>
       <c r="F193" s="8"/>
-      <c r="G193" s="21"/>
+      <c r="G193" s="20"/>
       <c r="H193" s="8"/>
       <c r="I193" s="8"/>
       <c r="J193" s="8"/>
@@ -7895,7 +7863,7 @@
       <c r="D194" s="8"/>
       <c r="E194" s="8"/>
       <c r="F194" s="8"/>
-      <c r="G194" s="21"/>
+      <c r="G194" s="20"/>
       <c r="H194" s="8"/>
       <c r="I194" s="8"/>
       <c r="J194" s="8"/>
@@ -7927,7 +7895,7 @@
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
       <c r="F195" s="8"/>
-      <c r="G195" s="21"/>
+      <c r="G195" s="20"/>
       <c r="H195" s="8"/>
       <c r="I195" s="8"/>
       <c r="J195" s="8"/>
@@ -7959,7 +7927,7 @@
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
       <c r="F196" s="8"/>
-      <c r="G196" s="21"/>
+      <c r="G196" s="20"/>
       <c r="H196" s="8"/>
       <c r="I196" s="8"/>
       <c r="J196" s="8"/>
@@ -7991,7 +7959,7 @@
       <c r="D197" s="8"/>
       <c r="E197" s="8"/>
       <c r="F197" s="8"/>
-      <c r="G197" s="21"/>
+      <c r="G197" s="20"/>
       <c r="H197" s="8"/>
       <c r="I197" s="8"/>
       <c r="J197" s="8"/>
@@ -8023,7 +7991,7 @@
       <c r="D198" s="8"/>
       <c r="E198" s="8"/>
       <c r="F198" s="8"/>
-      <c r="G198" s="21"/>
+      <c r="G198" s="20"/>
       <c r="H198" s="8"/>
       <c r="I198" s="8"/>
       <c r="J198" s="8"/>
@@ -8055,7 +8023,7 @@
       <c r="D199" s="8"/>
       <c r="E199" s="8"/>
       <c r="F199" s="8"/>
-      <c r="G199" s="21"/>
+      <c r="G199" s="20"/>
       <c r="H199" s="8"/>
       <c r="I199" s="8"/>
       <c r="J199" s="8"/>
@@ -8087,7 +8055,7 @@
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
       <c r="F200" s="8"/>
-      <c r="G200" s="21"/>
+      <c r="G200" s="20"/>
       <c r="H200" s="8"/>
       <c r="I200" s="8"/>
       <c r="J200" s="8"/>
@@ -8119,7 +8087,7 @@
       <c r="D201" s="8"/>
       <c r="E201" s="8"/>
       <c r="F201" s="8"/>
-      <c r="G201" s="21"/>
+      <c r="G201" s="20"/>
       <c r="H201" s="8"/>
       <c r="I201" s="8"/>
       <c r="J201" s="8"/>
@@ -8151,7 +8119,7 @@
       <c r="D202" s="8"/>
       <c r="E202" s="8"/>
       <c r="F202" s="8"/>
-      <c r="G202" s="21"/>
+      <c r="G202" s="20"/>
       <c r="H202" s="8"/>
       <c r="I202" s="8"/>
       <c r="J202" s="8"/>
@@ -8183,7 +8151,7 @@
       <c r="D203" s="8"/>
       <c r="E203" s="8"/>
       <c r="F203" s="8"/>
-      <c r="G203" s="21"/>
+      <c r="G203" s="20"/>
       <c r="H203" s="8"/>
       <c r="I203" s="8"/>
       <c r="J203" s="8"/>
@@ -8215,7 +8183,7 @@
       <c r="D204" s="8"/>
       <c r="E204" s="8"/>
       <c r="F204" s="8"/>
-      <c r="G204" s="21"/>
+      <c r="G204" s="20"/>
       <c r="H204" s="8"/>
       <c r="I204" s="8"/>
       <c r="J204" s="8"/>
@@ -8247,7 +8215,7 @@
       <c r="D205" s="8"/>
       <c r="E205" s="8"/>
       <c r="F205" s="8"/>
-      <c r="G205" s="21"/>
+      <c r="G205" s="20"/>
       <c r="H205" s="8"/>
       <c r="I205" s="8"/>
       <c r="J205" s="8"/>
@@ -8279,7 +8247,7 @@
       <c r="D206" s="8"/>
       <c r="E206" s="8"/>
       <c r="F206" s="8"/>
-      <c r="G206" s="21"/>
+      <c r="G206" s="20"/>
       <c r="H206" s="8"/>
       <c r="I206" s="8"/>
       <c r="J206" s="8"/>
@@ -8311,7 +8279,7 @@
       <c r="D207" s="8"/>
       <c r="E207" s="8"/>
       <c r="F207" s="8"/>
-      <c r="G207" s="21"/>
+      <c r="G207" s="20"/>
       <c r="H207" s="8"/>
       <c r="I207" s="8"/>
       <c r="J207" s="8"/>
@@ -8343,7 +8311,7 @@
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
       <c r="F208" s="8"/>
-      <c r="G208" s="21"/>
+      <c r="G208" s="20"/>
       <c r="H208" s="8"/>
       <c r="I208" s="8"/>
       <c r="J208" s="8"/>
@@ -8375,7 +8343,7 @@
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
       <c r="F209" s="8"/>
-      <c r="G209" s="21"/>
+      <c r="G209" s="20"/>
       <c r="H209" s="8"/>
       <c r="I209" s="8"/>
       <c r="J209" s="8"/>
@@ -8407,7 +8375,7 @@
       <c r="D210" s="8"/>
       <c r="E210" s="8"/>
       <c r="F210" s="8"/>
-      <c r="G210" s="21"/>
+      <c r="G210" s="20"/>
       <c r="H210" s="8"/>
       <c r="I210" s="8"/>
       <c r="J210" s="8"/>
@@ -8439,7 +8407,7 @@
       <c r="D211" s="8"/>
       <c r="E211" s="8"/>
       <c r="F211" s="8"/>
-      <c r="G211" s="21"/>
+      <c r="G211" s="20"/>
       <c r="H211" s="8"/>
       <c r="I211" s="8"/>
       <c r="J211" s="8"/>
@@ -8471,7 +8439,7 @@
       <c r="D212" s="8"/>
       <c r="E212" s="8"/>
       <c r="F212" s="8"/>
-      <c r="G212" s="21"/>
+      <c r="G212" s="20"/>
       <c r="H212" s="8"/>
       <c r="I212" s="8"/>
       <c r="J212" s="8"/>
@@ -8503,7 +8471,7 @@
       <c r="D213" s="8"/>
       <c r="E213" s="8"/>
       <c r="F213" s="8"/>
-      <c r="G213" s="21"/>
+      <c r="G213" s="20"/>
       <c r="H213" s="8"/>
       <c r="I213" s="8"/>
       <c r="J213" s="8"/>
@@ -8535,7 +8503,7 @@
       <c r="D214" s="8"/>
       <c r="E214" s="8"/>
       <c r="F214" s="8"/>
-      <c r="G214" s="21"/>
+      <c r="G214" s="20"/>
       <c r="H214" s="8"/>
       <c r="I214" s="8"/>
       <c r="J214" s="8"/>
@@ -8567,7 +8535,7 @@
       <c r="D215" s="8"/>
       <c r="E215" s="8"/>
       <c r="F215" s="8"/>
-      <c r="G215" s="21"/>
+      <c r="G215" s="20"/>
       <c r="H215" s="8"/>
       <c r="I215" s="8"/>
       <c r="J215" s="8"/>
@@ -8599,7 +8567,7 @@
       <c r="D216" s="8"/>
       <c r="E216" s="8"/>
       <c r="F216" s="8"/>
-      <c r="G216" s="21"/>
+      <c r="G216" s="20"/>
       <c r="H216" s="8"/>
       <c r="I216" s="8"/>
       <c r="J216" s="8"/>
@@ -8631,7 +8599,7 @@
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
       <c r="F217" s="8"/>
-      <c r="G217" s="21"/>
+      <c r="G217" s="20"/>
       <c r="H217" s="8"/>
       <c r="I217" s="8"/>
       <c r="J217" s="8"/>
@@ -8663,7 +8631,7 @@
       <c r="D218" s="8"/>
       <c r="E218" s="8"/>
       <c r="F218" s="8"/>
-      <c r="G218" s="21"/>
+      <c r="G218" s="20"/>
       <c r="H218" s="8"/>
       <c r="I218" s="8"/>
       <c r="J218" s="8"/>
@@ -8695,7 +8663,7 @@
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
       <c r="F219" s="8"/>
-      <c r="G219" s="21"/>
+      <c r="G219" s="20"/>
       <c r="H219" s="8"/>
       <c r="I219" s="8"/>
       <c r="J219" s="8"/>
@@ -8727,7 +8695,7 @@
       <c r="D220" s="8"/>
       <c r="E220" s="8"/>
       <c r="F220" s="8"/>
-      <c r="G220" s="21"/>
+      <c r="G220" s="20"/>
       <c r="H220" s="8"/>
       <c r="I220" s="8"/>
       <c r="J220" s="8"/>
@@ -8759,7 +8727,7 @@
       <c r="D221" s="8"/>
       <c r="E221" s="8"/>
       <c r="F221" s="8"/>
-      <c r="G221" s="21"/>
+      <c r="G221" s="20"/>
       <c r="H221" s="8"/>
       <c r="I221" s="8"/>
       <c r="J221" s="8"/>
@@ -8791,7 +8759,7 @@
       <c r="D222" s="8"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8"/>
-      <c r="G222" s="21"/>
+      <c r="G222" s="20"/>
       <c r="H222" s="8"/>
       <c r="I222" s="8"/>
       <c r="J222" s="8"/>
@@ -8823,7 +8791,7 @@
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
       <c r="F223" s="8"/>
-      <c r="G223" s="21"/>
+      <c r="G223" s="20"/>
       <c r="H223" s="8"/>
       <c r="I223" s="8"/>
       <c r="J223" s="8"/>
@@ -8855,7 +8823,7 @@
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
       <c r="F224" s="8"/>
-      <c r="G224" s="21"/>
+      <c r="G224" s="20"/>
       <c r="H224" s="8"/>
       <c r="I224" s="8"/>
       <c r="J224" s="8"/>
@@ -8887,7 +8855,7 @@
       <c r="D225" s="8"/>
       <c r="E225" s="8"/>
       <c r="F225" s="8"/>
-      <c r="G225" s="21"/>
+      <c r="G225" s="20"/>
       <c r="H225" s="8"/>
       <c r="I225" s="8"/>
       <c r="J225" s="8"/>
@@ -8919,7 +8887,7 @@
       <c r="D226" s="8"/>
       <c r="E226" s="8"/>
       <c r="F226" s="8"/>
-      <c r="G226" s="21"/>
+      <c r="G226" s="20"/>
       <c r="H226" s="8"/>
       <c r="I226" s="8"/>
       <c r="J226" s="8"/>
@@ -8951,7 +8919,7 @@
       <c r="D227" s="8"/>
       <c r="E227" s="8"/>
       <c r="F227" s="8"/>
-      <c r="G227" s="21"/>
+      <c r="G227" s="20"/>
       <c r="H227" s="8"/>
       <c r="I227" s="8"/>
       <c r="J227" s="8"/>
@@ -8983,7 +8951,7 @@
       <c r="D228" s="8"/>
       <c r="E228" s="8"/>
       <c r="F228" s="8"/>
-      <c r="G228" s="21"/>
+      <c r="G228" s="20"/>
       <c r="H228" s="8"/>
       <c r="I228" s="8"/>
       <c r="J228" s="8"/>
@@ -9015,7 +8983,7 @@
       <c r="D229" s="8"/>
       <c r="E229" s="8"/>
       <c r="F229" s="8"/>
-      <c r="G229" s="21"/>
+      <c r="G229" s="20"/>
       <c r="H229" s="8"/>
       <c r="I229" s="8"/>
       <c r="J229" s="8"/>
@@ -9047,7 +9015,7 @@
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
       <c r="F230" s="8"/>
-      <c r="G230" s="21"/>
+      <c r="G230" s="20"/>
       <c r="H230" s="8"/>
       <c r="I230" s="8"/>
       <c r="J230" s="8"/>
@@ -9079,7 +9047,7 @@
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
       <c r="F231" s="8"/>
-      <c r="G231" s="21"/>
+      <c r="G231" s="20"/>
       <c r="H231" s="8"/>
       <c r="I231" s="8"/>
       <c r="J231" s="8"/>
@@ -9111,7 +9079,7 @@
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
       <c r="F232" s="8"/>
-      <c r="G232" s="21"/>
+      <c r="G232" s="20"/>
       <c r="H232" s="8"/>
       <c r="I232" s="8"/>
       <c r="J232" s="8"/>
@@ -9143,7 +9111,7 @@
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
       <c r="F233" s="8"/>
-      <c r="G233" s="21"/>
+      <c r="G233" s="20"/>
       <c r="H233" s="8"/>
       <c r="I233" s="8"/>
       <c r="J233" s="8"/>
@@ -9175,7 +9143,7 @@
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
       <c r="F234" s="8"/>
-      <c r="G234" s="21"/>
+      <c r="G234" s="20"/>
       <c r="H234" s="8"/>
       <c r="I234" s="8"/>
       <c r="J234" s="8"/>
@@ -9207,7 +9175,7 @@
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
       <c r="F235" s="8"/>
-      <c r="G235" s="21"/>
+      <c r="G235" s="20"/>
       <c r="H235" s="8"/>
       <c r="I235" s="8"/>
       <c r="J235" s="8"/>
@@ -9239,7 +9207,7 @@
       <c r="D236" s="8"/>
       <c r="E236" s="8"/>
       <c r="F236" s="8"/>
-      <c r="G236" s="21"/>
+      <c r="G236" s="20"/>
       <c r="H236" s="8"/>
       <c r="I236" s="8"/>
       <c r="J236" s="8"/>
@@ -9271,7 +9239,7 @@
       <c r="D237" s="8"/>
       <c r="E237" s="8"/>
       <c r="F237" s="8"/>
-      <c r="G237" s="21"/>
+      <c r="G237" s="20"/>
       <c r="H237" s="8"/>
       <c r="I237" s="8"/>
       <c r="J237" s="8"/>
@@ -9303,7 +9271,7 @@
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
       <c r="F238" s="8"/>
-      <c r="G238" s="21"/>
+      <c r="G238" s="20"/>
       <c r="H238" s="8"/>
       <c r="I238" s="8"/>
       <c r="J238" s="8"/>
@@ -9335,7 +9303,7 @@
       <c r="D239" s="8"/>
       <c r="E239" s="8"/>
       <c r="F239" s="8"/>
-      <c r="G239" s="21"/>
+      <c r="G239" s="20"/>
       <c r="H239" s="8"/>
       <c r="I239" s="8"/>
       <c r="J239" s="8"/>
@@ -33581,14 +33549,13 @@
     <hyperlink ref="H30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="H31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="H32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="H35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="H36" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="H37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H9" r:id="rId32" display="https://www.mouser.ch/ProductDetail/Amphenol-FCI/67996-420HLF?qs=QKvFUfBIyQIvQWWcVN8Heg%3D%3D" xr:uid="{76DDBB45-968B-48DB-9A14-6A41AF7AA4FF}"/>
-    <hyperlink ref="H19" r:id="rId33" display="https://www.mouser.ch/ProductDetail/Amphenol-FCI/10129381-940002BLF?qs=0lQeLiL1qybDkBpXY7DYcQ%3D%3D" xr:uid="{9842B8A2-D326-405F-81E9-8F16BB31F05D}"/>
+    <hyperlink ref="H35" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H36" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H37" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H9" r:id="rId31" display="https://www.mouser.ch/ProductDetail/Amphenol-FCI/67996-420HLF?qs=QKvFUfBIyQIvQWWcVN8Heg%3D%3D" xr:uid="{76DDBB45-968B-48DB-9A14-6A41AF7AA4FF}"/>
+    <hyperlink ref="H19" r:id="rId32" display="https://www.mouser.ch/ProductDetail/Amphenol-FCI/10129381-940002BLF?qs=0lQeLiL1qybDkBpXY7DYcQ%3D%3D" xr:uid="{9842B8A2-D326-405F-81E9-8F16BB31F05D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>